<commit_message>
#165 point score calculation logic improvement
</commit_message>
<xml_diff>
--- a/src/main/data/IPL-2019-Venue.xlsx
+++ b/src/main/data/IPL-2019-Venue.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/repo/Sport-fantasy-league/src/main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B0F0AA-D96B-6247-B33D-95D260A46DE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338CCE8A-D477-0C4C-915D-A11E6FD38EE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9782549C-49E7-5541-8E84-13FD309B38D6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16220" xr2:uid="{9782549C-49E7-5541-8E84-13FD309B38D6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>M. A. Chidambaram Stadium</t>
   </si>
@@ -76,6 +77,18 @@
   </si>
   <si>
     <t>BENGALURE</t>
+  </si>
+  <si>
+    <t>ABU DHABI</t>
+  </si>
+  <si>
+    <t>DUBAI</t>
+  </si>
+  <si>
+    <t>SHARJAH</t>
+  </si>
+  <si>
+    <t>UAE</t>
   </si>
 </sst>
 </file>
@@ -440,11 +453,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57E5A4E-B54E-3942-93A7-00D2A1774017}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95526E9-4363-F641-A70F-AC898BB51718}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
#195 adding changes for production readiness
</commit_message>
<xml_diff>
--- a/src/main/data/IPL-2019-Venue.xlsx
+++ b/src/main/data/IPL-2019-Venue.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/repo/Sport-fantasy-league/src/main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338CCE8A-D477-0C4C-915D-A11E6FD38EE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3375DA32-D443-974B-93E6-A4B3A2E40C8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16220" xr2:uid="{9782549C-49E7-5541-8E84-13FD309B38D6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>M. A. Chidambaram Stadium</t>
   </si>
@@ -37,9 +37,6 @@
     <t>INDIA</t>
   </si>
   <si>
-    <t>Feroz Shah Kotla</t>
-  </si>
-  <si>
     <t>DELHI</t>
   </si>
   <si>
@@ -89,6 +86,15 @@
   </si>
   <si>
     <t>UAE</t>
+  </si>
+  <si>
+    <t>Narendra Modi Stadium</t>
+  </si>
+  <si>
+    <t>Ahmedabad</t>
+  </si>
+  <si>
+    <t>Arun Jaitley Stadium</t>
   </si>
 </sst>
 </file>
@@ -453,10 +459,128 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95526E9-4363-F641-A70F-AC898BB51718}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.33203125" customWidth="1"/>
+    <col min="2" max="2" width="48.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57E5A4E-B54E-3942-93A7-00D2A1774017}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -468,142 +592,35 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95526E9-4363-F641-A70F-AC898BB51718}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="37.33203125" customWidth="1"/>
-    <col min="2" max="2" width="48.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>